<commit_message>
Switched TextBox and both NumericUpDown control properties "Enable" and "ReadOnly" from "false" to "true".
</commit_message>
<xml_diff>
--- a/Snake/Documents/Helper.xlsx
+++ b/Snake/Documents/Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Visual Studio Projects\Visual Studio 2019\Projetcs\Snake\Snake\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA1C81-52EE-46AD-9AE4-19A7756267F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F24266-D8C6-4453-8C5E-9D09388BB279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{43A73AA5-ABFD-421F-BFC1-09D3FBCE3DF0}"/>
   </bookViews>
@@ -1161,12 +1161,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -1191,6 +1185,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13667,8 +13667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7C1CA8-4445-4A42-837E-08649278B969}">
   <dimension ref="A8:BS163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="BF122" sqref="BF122"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="N105" sqref="N105:O106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -15844,33 +15844,33 @@
         <f t="shared" ref="AD67" si="29">AC67+1</f>
         <v>5</v>
       </c>
-      <c r="AM67" s="109"/>
-      <c r="AN67" s="110">
+      <c r="AM67" s="107"/>
+      <c r="AN67" s="108">
         <v>1</v>
       </c>
-      <c r="AO67" s="110">
+      <c r="AO67" s="108">
         <f>AN67+1</f>
         <v>2</v>
       </c>
-      <c r="AP67" s="110">
+      <c r="AP67" s="108">
         <f>AO67+1</f>
         <v>3</v>
       </c>
-      <c r="AQ67" s="110">
+      <c r="AQ67" s="108">
         <f>AP67+1</f>
         <v>4</v>
       </c>
-      <c r="AR67" s="110">
+      <c r="AR67" s="108">
         <f>AQ67+1</f>
         <v>5</v>
       </c>
-      <c r="AS67" s="110">
+      <c r="AS67" s="108">
         <f>AR67+1</f>
         <v>6</v>
       </c>
-      <c r="AT67" s="111"/>
-      <c r="AU67" s="111"/>
-      <c r="AV67" s="112"/>
+      <c r="AT67" s="109"/>
+      <c r="AU67" s="109"/>
+      <c r="AV67" s="110"/>
     </row>
     <row r="68" spans="25:65">
       <c r="Y68" s="1">
@@ -15891,7 +15891,7 @@
       <c r="AD68" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AM68" s="113">
+      <c r="AM68" s="111">
         <v>1</v>
       </c>
       <c r="AN68" s="16" t="s">
@@ -15945,7 +15945,7 @@
       <c r="AD69" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AM69" s="113">
+      <c r="AM69" s="111">
         <f>AM68+1</f>
         <v>2</v>
       </c>
@@ -16000,7 +16000,7 @@
       <c r="AD70" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AM70" s="113">
+      <c r="AM70" s="111">
         <f>AM69+1</f>
         <v>3</v>
       </c>
@@ -16046,7 +16046,7 @@
       <c r="AD71" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AM71" s="113">
+      <c r="AM71" s="111">
         <f>AM70+1</f>
         <v>4</v>
       </c>
@@ -16123,7 +16123,7 @@
         <f t="shared" ref="AD74" si="32">AC74+1</f>
         <v>5</v>
       </c>
-      <c r="AM74" s="114"/>
+      <c r="AM74" s="112"/>
       <c r="AN74" s="5">
         <v>1</v>
       </c>
@@ -16170,7 +16170,7 @@
       <c r="AD75" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AM75" s="113">
+      <c r="AM75" s="111">
         <v>1</v>
       </c>
       <c r="AN75" s="15" t="s">
@@ -16215,7 +16215,7 @@
       <c r="AD76" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AM76" s="113">
+      <c r="AM76" s="111">
         <f>AM75+1</f>
         <v>2</v>
       </c>
@@ -16261,7 +16261,7 @@
       <c r="AD77" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AM77" s="113">
+      <c r="AM77" s="111">
         <f>AM76+1</f>
         <v>3</v>
       </c>
@@ -16307,7 +16307,7 @@
       <c r="AD78" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AM78" s="113">
+      <c r="AM78" s="111">
         <f>AM77+1</f>
         <v>4</v>
       </c>
@@ -16374,7 +16374,7 @@
       <c r="AV81" s="89"/>
     </row>
     <row r="82" spans="39:48">
-      <c r="AM82" s="114"/>
+      <c r="AM82" s="112"/>
       <c r="AN82" s="2"/>
       <c r="AO82" s="2"/>
       <c r="AP82" s="2"/>
@@ -16383,7 +16383,7 @@
       <c r="AS82" s="2"/>
       <c r="AT82" s="2"/>
       <c r="AU82" s="2"/>
-      <c r="AV82" s="115"/>
+      <c r="AV82" s="113"/>
     </row>
     <row r="84" spans="39:48">
       <c r="AN84" t="s">
@@ -16623,27 +16623,27 @@
       <c r="Y103" t="s">
         <v>128</v>
       </c>
-      <c r="AQ103" s="123"/>
-      <c r="AR103" s="124"/>
-      <c r="AS103" s="124"/>
-      <c r="AT103" s="124"/>
-      <c r="AU103" s="124"/>
-      <c r="AV103" s="124"/>
-      <c r="AW103" s="124"/>
-      <c r="AX103" s="124"/>
-      <c r="AY103" s="124"/>
-      <c r="AZ103" s="124"/>
-      <c r="BA103" s="124"/>
-      <c r="BB103" s="124"/>
-      <c r="BC103" s="124"/>
-      <c r="BD103" s="124"/>
-      <c r="BE103" s="124"/>
-      <c r="BF103" s="124"/>
-      <c r="BG103" s="124"/>
-      <c r="BH103" s="124"/>
-      <c r="BI103" s="124"/>
-      <c r="BJ103" s="124"/>
-      <c r="BK103" s="124"/>
+      <c r="AQ103" s="121"/>
+      <c r="AR103" s="122"/>
+      <c r="AS103" s="122"/>
+      <c r="AT103" s="122"/>
+      <c r="AU103" s="122"/>
+      <c r="AV103" s="122"/>
+      <c r="AW103" s="122"/>
+      <c r="AX103" s="122"/>
+      <c r="AY103" s="122"/>
+      <c r="AZ103" s="122"/>
+      <c r="BA103" s="122"/>
+      <c r="BB103" s="122"/>
+      <c r="BC103" s="122"/>
+      <c r="BD103" s="122"/>
+      <c r="BE103" s="122"/>
+      <c r="BF103" s="122"/>
+      <c r="BG103" s="122"/>
+      <c r="BH103" s="122"/>
+      <c r="BI103" s="122"/>
+      <c r="BJ103" s="122"/>
+      <c r="BK103" s="122"/>
       <c r="BL103" s="13"/>
     </row>
     <row r="104" spans="3:71" ht="15" thickBot="1">
@@ -16707,19 +16707,19 @@
       <c r="Z104" s="5">
         <v>1</v>
       </c>
-      <c r="AA104" s="119">
+      <c r="AA104" s="117">
         <f>Z104+1</f>
         <v>2</v>
       </c>
-      <c r="AB104" s="120">
+      <c r="AB104" s="118">
         <f>AA104+1</f>
         <v>3</v>
       </c>
-      <c r="AC104" s="119">
+      <c r="AC104" s="117">
         <f>AB104+1</f>
         <v>4</v>
       </c>
-      <c r="AD104" s="120">
+      <c r="AD104" s="118">
         <f>AC104+1</f>
         <v>5</v>
       </c>
@@ -16732,27 +16732,27 @@
         <v>1</v>
       </c>
       <c r="AI104" s="5">
-        <f>AH104+1</f>
+        <f t="shared" ref="AI104:AN104" si="35">AH104+1</f>
         <v>2</v>
       </c>
       <c r="AJ104" s="5">
-        <f>AI104+1</f>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="AK104" s="5">
-        <f>AJ104+1</f>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="AL104" s="5">
-        <f>AK104+1</f>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="AM104" s="5">
-        <f>AL104+1</f>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="AN104" s="5">
-        <f>AM104+1</f>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="AQ104" s="20"/>
@@ -16786,7 +16786,7 @@
       <c r="BI104" s="21"/>
       <c r="BJ104" s="21"/>
       <c r="BK104" s="21"/>
-      <c r="BL104" s="125">
+      <c r="BL104" s="123">
         <f>BE104+1</f>
         <v>4</v>
       </c>
@@ -16852,16 +16852,16 @@
       <c r="Z105" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AA105" s="121" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB105" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC105" s="121" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD105" s="122" t="s">
+      <c r="AA105" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB105" s="120" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC105" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD105" s="120" t="s">
         <v>13</v>
       </c>
       <c r="AE105" s="9" t="s">
@@ -16924,7 +16924,7 @@
       <c r="BI105" s="21"/>
       <c r="BJ105" s="21"/>
       <c r="BK105" s="21"/>
-      <c r="BL105" s="122" t="s">
+      <c r="BL105" s="120" t="s">
         <v>13</v>
       </c>
       <c r="BP105" t="s">
@@ -16934,7 +16934,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="3:71">
+    <row r="106" spans="3:71" ht="15" thickBot="1">
       <c r="C106" s="1">
         <f>C105+1</f>
         <v>2</v>
@@ -16965,10 +16965,10 @@
       <c r="M106" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N106" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="O106" s="116" t="s">
+      <c r="N106" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="O106" s="126" t="s">
         <v>15</v>
       </c>
       <c r="P106" s="8" t="s">
@@ -17003,13 +17003,13 @@
       <c r="AA106" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AB106" s="116" t="s">
+      <c r="AB106" s="114" t="s">
         <v>15</v>
       </c>
       <c r="AC106" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AD106" s="116" t="s">
+      <c r="AD106" s="114" t="s">
         <v>15</v>
       </c>
       <c r="AE106" s="8" t="s">
@@ -17060,7 +17060,7 @@
       <c r="BD106" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="BE106" s="116" t="s">
+      <c r="BE106" s="114" t="s">
         <v>15</v>
       </c>
       <c r="BF106" s="21"/>
@@ -17069,7 +17069,7 @@
       <c r="BI106" s="21"/>
       <c r="BJ106" s="21"/>
       <c r="BK106" s="21"/>
-      <c r="BL106" s="126" t="s">
+      <c r="BL106" s="124" t="s">
         <v>16</v>
       </c>
       <c r="BN106" t="s">
@@ -17113,10 +17113,10 @@
       <c r="M107" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N107" s="117" t="s">
+      <c r="N107" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="O107" s="118" t="s">
+      <c r="O107" s="116" t="s">
         <v>17</v>
       </c>
       <c r="P107" s="8" t="s">
@@ -17148,16 +17148,16 @@
       <c r="Z107" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AA107" s="117" t="s">
+      <c r="AA107" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="AB107" s="118" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC107" s="117" t="s">
+      <c r="AB107" s="116" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC107" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="AD107" s="118" t="s">
+      <c r="AD107" s="116" t="s">
         <v>17</v>
       </c>
       <c r="AE107" s="8" t="s">
@@ -17205,10 +17205,10 @@
       <c r="BA107" s="21"/>
       <c r="BB107" s="21"/>
       <c r="BC107" s="21"/>
-      <c r="BD107" s="117" t="s">
+      <c r="BD107" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="BE107" s="118" t="s">
+      <c r="BE107" s="116" t="s">
         <v>17</v>
       </c>
       <c r="BF107" s="21"/>
@@ -17217,7 +17217,7 @@
       <c r="BI107" s="21"/>
       <c r="BJ107" s="21"/>
       <c r="BK107" s="21"/>
-      <c r="BL107" s="126" t="s">
+      <c r="BL107" s="124" t="s">
         <v>16</v>
       </c>
     </row>
@@ -17535,10 +17535,10 @@
       <c r="M116" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N116" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="O116" s="128" t="s">
+      <c r="N116" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="O116" s="126" t="s">
         <v>15</v>
       </c>
       <c r="P116" s="8" t="s">
@@ -17551,16 +17551,16 @@
       <c r="Z116" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AA116" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB116" s="128" t="s">
+      <c r="AA116" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB116" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="AC116" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD116" s="128" t="s">
+      <c r="AC116" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD116" s="126" t="s">
         <v>15</v>
       </c>
       <c r="AE116" s="8" t="s">
@@ -17585,10 +17585,10 @@
       <c r="M117" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N117" s="131" t="s">
+      <c r="N117" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="O117" s="132" t="s">
+      <c r="O117" s="130" t="s">
         <v>15</v>
       </c>
       <c r="P117" s="8" t="s">
@@ -17601,16 +17601,16 @@
       <c r="Z117" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AA117" s="131" t="s">
+      <c r="AA117" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="AB117" s="132" t="s">
+      <c r="AB117" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="AC117" s="131" t="s">
+      <c r="AC117" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="AD117" s="132" t="s">
+      <c r="AD117" s="130" t="s">
         <v>15</v>
       </c>
       <c r="AE117" s="8" t="s">
@@ -17645,10 +17645,10 @@
       <c r="M118" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N118" s="117" t="s">
+      <c r="N118" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="O118" s="128" t="s">
+      <c r="O118" s="126" t="s">
         <v>15</v>
       </c>
       <c r="P118" s="8" t="s">
@@ -17661,16 +17661,16 @@
       <c r="Z118" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AA118" s="117" t="s">
+      <c r="AA118" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="AB118" s="128" t="s">
+      <c r="AB118" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="AC118" s="117" t="s">
+      <c r="AC118" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="AD118" s="128" t="s">
+      <c r="AD118" s="126" t="s">
         <v>15</v>
       </c>
       <c r="AE118" s="8" t="s">
@@ -17707,10 +17707,10 @@
       <c r="M119" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N119" s="129" t="s">
+      <c r="N119" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="O119" s="130" t="s">
+      <c r="O119" s="128" t="s">
         <v>17</v>
       </c>
       <c r="P119" s="8" t="s">
@@ -17723,16 +17723,16 @@
       <c r="Z119" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AA119" s="129" t="s">
+      <c r="AA119" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="AB119" s="130" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC119" s="129" t="s">
+      <c r="AB119" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC119" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="AD119" s="130" t="s">
+      <c r="AD119" s="128" t="s">
         <v>17</v>
       </c>
       <c r="AE119" s="8" t="s">
@@ -17784,65 +17784,65 @@
     </row>
     <row r="133" spans="2:61" ht="15" thickBot="1"/>
     <row r="134" spans="2:61">
-      <c r="B134" s="123"/>
-      <c r="C134" s="124"/>
-      <c r="D134" s="124"/>
-      <c r="E134" s="124"/>
-      <c r="F134" s="124"/>
-      <c r="G134" s="124"/>
-      <c r="H134" s="124"/>
-      <c r="I134" s="124"/>
-      <c r="J134" s="124"/>
-      <c r="K134" s="124"/>
-      <c r="L134" s="124"/>
-      <c r="M134" s="124"/>
-      <c r="N134" s="124"/>
-      <c r="O134" s="124"/>
-      <c r="P134" s="124"/>
-      <c r="Q134" s="124"/>
-      <c r="R134" s="124"/>
-      <c r="S134" s="124"/>
-      <c r="T134" s="124"/>
-      <c r="U134" s="124"/>
-      <c r="V134" s="124"/>
-      <c r="W134" s="124"/>
-      <c r="X134" s="124"/>
-      <c r="Y134" s="124"/>
-      <c r="Z134" s="124"/>
-      <c r="AA134" s="124"/>
-      <c r="AB134" s="124"/>
-      <c r="AC134" s="124"/>
-      <c r="AD134" s="124"/>
-      <c r="AE134" s="124"/>
-      <c r="AF134" s="124"/>
-      <c r="AG134" s="124"/>
-      <c r="AH134" s="124"/>
-      <c r="AI134" s="124"/>
-      <c r="AJ134" s="124"/>
-      <c r="AK134" s="124"/>
-      <c r="AL134" s="124"/>
-      <c r="AM134" s="124"/>
-      <c r="AN134" s="124"/>
-      <c r="AO134" s="124"/>
-      <c r="AP134" s="124"/>
-      <c r="AQ134" s="124"/>
-      <c r="AR134" s="124"/>
-      <c r="AS134" s="124"/>
-      <c r="AT134" s="124"/>
-      <c r="AU134" s="124"/>
-      <c r="AV134" s="124"/>
-      <c r="AW134" s="124"/>
-      <c r="AX134" s="124"/>
-      <c r="AY134" s="124"/>
-      <c r="AZ134" s="124"/>
-      <c r="BA134" s="124"/>
-      <c r="BB134" s="124"/>
-      <c r="BC134" s="124"/>
-      <c r="BD134" s="124"/>
-      <c r="BE134" s="124"/>
-      <c r="BF134" s="124"/>
-      <c r="BG134" s="124"/>
-      <c r="BH134" s="124"/>
+      <c r="B134" s="121"/>
+      <c r="C134" s="122"/>
+      <c r="D134" s="122"/>
+      <c r="E134" s="122"/>
+      <c r="F134" s="122"/>
+      <c r="G134" s="122"/>
+      <c r="H134" s="122"/>
+      <c r="I134" s="122"/>
+      <c r="J134" s="122"/>
+      <c r="K134" s="122"/>
+      <c r="L134" s="122"/>
+      <c r="M134" s="122"/>
+      <c r="N134" s="122"/>
+      <c r="O134" s="122"/>
+      <c r="P134" s="122"/>
+      <c r="Q134" s="122"/>
+      <c r="R134" s="122"/>
+      <c r="S134" s="122"/>
+      <c r="T134" s="122"/>
+      <c r="U134" s="122"/>
+      <c r="V134" s="122"/>
+      <c r="W134" s="122"/>
+      <c r="X134" s="122"/>
+      <c r="Y134" s="122"/>
+      <c r="Z134" s="122"/>
+      <c r="AA134" s="122"/>
+      <c r="AB134" s="122"/>
+      <c r="AC134" s="122"/>
+      <c r="AD134" s="122"/>
+      <c r="AE134" s="122"/>
+      <c r="AF134" s="122"/>
+      <c r="AG134" s="122"/>
+      <c r="AH134" s="122"/>
+      <c r="AI134" s="122"/>
+      <c r="AJ134" s="122"/>
+      <c r="AK134" s="122"/>
+      <c r="AL134" s="122"/>
+      <c r="AM134" s="122"/>
+      <c r="AN134" s="122"/>
+      <c r="AO134" s="122"/>
+      <c r="AP134" s="122"/>
+      <c r="AQ134" s="122"/>
+      <c r="AR134" s="122"/>
+      <c r="AS134" s="122"/>
+      <c r="AT134" s="122"/>
+      <c r="AU134" s="122"/>
+      <c r="AV134" s="122"/>
+      <c r="AW134" s="122"/>
+      <c r="AX134" s="122"/>
+      <c r="AY134" s="122"/>
+      <c r="AZ134" s="122"/>
+      <c r="BA134" s="122"/>
+      <c r="BB134" s="122"/>
+      <c r="BC134" s="122"/>
+      <c r="BD134" s="122"/>
+      <c r="BE134" s="122"/>
+      <c r="BF134" s="122"/>
+      <c r="BG134" s="122"/>
+      <c r="BH134" s="122"/>
       <c r="BI134" s="13"/>
     </row>
     <row r="135" spans="2:61">
@@ -20235,25 +20235,25 @@
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
-      <c r="K10" s="108"/>
-      <c r="L10" s="108"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="132"/>
       <c r="V10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="131" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="26"/>
@@ -20301,7 +20301,7 @@
       </c>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="107"/>
+      <c r="A12" s="131"/>
       <c r="B12" s="28">
         <v>0</v>
       </c>
@@ -20340,7 +20340,7 @@
       </c>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="107"/>
+      <c r="A13" s="131"/>
       <c r="B13" s="28">
         <f t="shared" ref="B13:B18" si="2">B12+1</f>
         <v>1</v>
@@ -20377,7 +20377,7 @@
       </c>
     </row>
     <row r="14" spans="1:29">
-      <c r="A14" s="107"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="28">
         <f t="shared" si="2"/>
         <v>2</v>
@@ -20417,7 +20417,7 @@
       </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="107"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="28">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -20457,7 +20457,7 @@
       </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="107"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="28">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -20497,7 +20497,7 @@
       </c>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="107"/>
+      <c r="A17" s="131"/>
       <c r="B17" s="28">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -20534,7 +20534,7 @@
       </c>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="107"/>
+      <c r="A18" s="131"/>
       <c r="B18" s="28">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -20574,7 +20574,7 @@
       </c>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="107"/>
+      <c r="A19" s="131"/>
       <c r="B19" s="28">
         <f t="shared" ref="B19:B21" si="3">B18+1</f>
         <v>7</v>
@@ -20614,7 +20614,7 @@
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="107"/>
+      <c r="A20" s="131"/>
       <c r="B20" s="28">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -20651,7 +20651,7 @@
       </c>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="107"/>
+      <c r="A21" s="131"/>
       <c r="B21" s="28">
         <f t="shared" si="3"/>
         <v>9</v>

</xml_diff>

<commit_message>
Added some proerties to have more information available about the Hamiltonian Cycle.
</commit_message>
<xml_diff>
--- a/Snake/Documents/Helper.xlsx
+++ b/Snake/Documents/Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Visual Studio Projects\Visual Studio 2019\Projetcs\Snake\Snake\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B72A654-411D-41F7-8E1A-2BE53BB54EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A02DE4-1B3C-4059-9051-AE26EF79C8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{43A73AA5-ABFD-421F-BFC1-09D3FBCE3DF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="181">
   <si>
     <t>Hoehe</t>
   </si>
@@ -545,6 +545,45 @@
   <si>
     <t>where eaten!</t>
   </si>
+  <si>
+    <t xml:space="preserve">if true -&gt; </t>
+  </si>
+  <si>
+    <t>this set up would return false -&gt; no shortcut woul be caclulated!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all snake parts now in the hamiltonian cycle </t>
+  </si>
+  <si>
+    <t>areAllSnakePartsInTheHamiltonianCycle</t>
+  </si>
+  <si>
+    <t>is now equalt to true</t>
+  </si>
+  <si>
+    <t>und enthält das fett umrandete Feld keine snake parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = function (...)</t>
+  </si>
+  <si>
+    <t>eight move furhther:</t>
+  </si>
+  <si>
+    <t>Wennalle snake parts im Ham cycle sind, aknn</t>
+  </si>
+  <si>
+    <t>im fett umrahmte bereich (niemals!) kein snake part sein!</t>
+  </si>
+  <si>
+    <t>shortcut berechnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nur durchführen wenn </t>
+  </si>
+  <si>
+    <t>appl im fett umrahmten bereich ist.</t>
+  </si>
 </sst>
 </file>
 
@@ -615,7 +654,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,6 +742,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1238,7 +1283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1538,6 +1583,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10206,10 +10265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C7CDE-FA09-4542-9DD9-60A1EEECAB2D}">
-  <dimension ref="A2:AV150"/>
+  <dimension ref="A2:AX188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="J153" sqref="J153"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="AN174" sqref="AN174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -15248,6 +15307,11 @@
       <c r="AI132" s="2"/>
       <c r="AJ132" s="113"/>
     </row>
+    <row r="141" spans="2:36">
+      <c r="U141" t="s">
+        <v>171</v>
+      </c>
+    </row>
     <row r="142" spans="2:36">
       <c r="F142" s="2">
         <v>0</v>
@@ -15276,6 +15340,9 @@
         <f t="shared" si="44"/>
         <v>6</v>
       </c>
+      <c r="U142" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="143" spans="2:36">
       <c r="E143">
@@ -15283,6 +15350,9 @@
       </c>
       <c r="F143" s="137"/>
       <c r="L143" s="110"/>
+      <c r="V143" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="144" spans="2:36">
       <c r="E144">
@@ -15292,7 +15362,7 @@
       <c r="F144" s="138"/>
       <c r="L144" s="89"/>
     </row>
-    <row r="145" spans="5:12" ht="15" thickBot="1">
+    <row r="145" spans="5:32" ht="15" thickBot="1">
       <c r="E145">
         <f t="shared" si="45"/>
         <v>2</v>
@@ -15316,8 +15386,11 @@
       <c r="L145" s="140" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="146" spans="5:12">
+      <c r="U145" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="146" spans="5:32">
       <c r="E146">
         <f t="shared" si="45"/>
         <v>3</v>
@@ -15342,7 +15415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" spans="5:12">
+    <row r="147" spans="5:32">
       <c r="E147">
         <f t="shared" si="45"/>
         <v>4</v>
@@ -15351,23 +15424,11 @@
       <c r="G147" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H147" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I147" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J147" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K147" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L147" s="140" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="148" spans="5:12">
+      <c r="V147" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="148" spans="5:32">
       <c r="E148">
         <f t="shared" si="45"/>
         <v>5</v>
@@ -15391,8 +15452,47 @@
       <c r="L148" s="141" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="149" spans="5:12">
+      <c r="W148" s="2">
+        <v>0</v>
+      </c>
+      <c r="X148" s="2">
+        <f t="shared" ref="X148" si="46">W148+1</f>
+        <v>1</v>
+      </c>
+      <c r="Y148" s="2">
+        <f t="shared" ref="Y148" si="47">X148+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z148" s="2">
+        <f t="shared" ref="Z148" si="48">Y148+1</f>
+        <v>3</v>
+      </c>
+      <c r="AA148" s="2">
+        <f t="shared" ref="AA148" si="49">Z148+1</f>
+        <v>4</v>
+      </c>
+      <c r="AB148" s="2">
+        <f t="shared" ref="AB148" si="50">AA148+1</f>
+        <v>5</v>
+      </c>
+      <c r="AC148" s="2">
+        <f t="shared" ref="AC148" si="51">AB148+1</f>
+        <v>6</v>
+      </c>
+      <c r="AD148" s="2">
+        <f t="shared" ref="AD148" si="52">AC148+1</f>
+        <v>7</v>
+      </c>
+      <c r="AE148" s="2">
+        <f t="shared" ref="AE148" si="53">AD148+1</f>
+        <v>8</v>
+      </c>
+      <c r="AF148" s="2">
+        <f t="shared" ref="AF148" si="54">AE148+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="5:32">
       <c r="E149">
         <f t="shared" si="45"/>
         <v>6</v>
@@ -15414,13 +15514,885 @@
       <c r="L149" s="140" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="150" spans="5:12">
+      <c r="V149">
+        <v>0</v>
+      </c>
+      <c r="W149" s="142"/>
+      <c r="X149" s="145"/>
+      <c r="Y149" s="145"/>
+      <c r="Z149" s="145"/>
+      <c r="AA149" s="145"/>
+      <c r="AB149" s="145"/>
+      <c r="AC149" s="145"/>
+      <c r="AD149" s="145"/>
+      <c r="AE149" s="145"/>
+      <c r="AF149" s="146"/>
+    </row>
+    <row r="150" spans="5:32">
       <c r="E150" t="s">
         <v>80</v>
       </c>
       <c r="F150" s="138"/>
       <c r="L150" s="89"/>
+      <c r="V150">
+        <f t="shared" ref="V150:V158" si="55">V149+1</f>
+        <v>1</v>
+      </c>
+      <c r="W150" s="143"/>
+      <c r="X150" s="147"/>
+      <c r="Y150" s="147"/>
+      <c r="Z150" s="147"/>
+      <c r="AA150" s="147"/>
+      <c r="AB150" s="147"/>
+      <c r="AC150" s="147"/>
+      <c r="AD150" s="147"/>
+      <c r="AE150" s="147"/>
+      <c r="AF150" s="148"/>
+    </row>
+    <row r="151" spans="5:32">
+      <c r="V151">
+        <f t="shared" si="55"/>
+        <v>2</v>
+      </c>
+      <c r="W151" s="143"/>
+      <c r="X151" s="147"/>
+      <c r="Y151" s="147"/>
+      <c r="Z151" s="147"/>
+      <c r="AA151" s="147"/>
+      <c r="AB151" s="147" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC151" s="21"/>
+      <c r="AD151" s="21"/>
+      <c r="AE151" s="21"/>
+      <c r="AF151" s="89"/>
+    </row>
+    <row r="152" spans="5:32">
+      <c r="V152">
+        <f t="shared" si="55"/>
+        <v>3</v>
+      </c>
+      <c r="W152" s="143"/>
+      <c r="X152" s="21"/>
+      <c r="Y152" s="74"/>
+      <c r="Z152" s="21"/>
+      <c r="AA152" s="21"/>
+      <c r="AB152" s="147">
+        <v>8</v>
+      </c>
+      <c r="AC152" s="21"/>
+      <c r="AD152" s="21"/>
+      <c r="AE152" s="21"/>
+      <c r="AF152" s="89"/>
+    </row>
+    <row r="153" spans="5:32">
+      <c r="V153">
+        <f t="shared" si="55"/>
+        <v>4</v>
+      </c>
+      <c r="W153" s="143"/>
+      <c r="X153" s="21"/>
+      <c r="Y153" s="21"/>
+      <c r="Z153" s="21"/>
+      <c r="AA153" s="21"/>
+      <c r="AB153" s="147">
+        <v>7</v>
+      </c>
+      <c r="AC153" s="21"/>
+      <c r="AD153" s="21"/>
+      <c r="AE153" s="21"/>
+      <c r="AF153" s="89"/>
+    </row>
+    <row r="154" spans="5:32">
+      <c r="V154">
+        <f t="shared" si="55"/>
+        <v>5</v>
+      </c>
+      <c r="W154" s="143"/>
+      <c r="X154" s="21"/>
+      <c r="Y154" s="21"/>
+      <c r="Z154" s="21"/>
+      <c r="AA154" s="21"/>
+      <c r="AB154" s="147">
+        <v>6</v>
+      </c>
+      <c r="AC154" s="21"/>
+      <c r="AD154" s="21"/>
+      <c r="AE154" s="21"/>
+      <c r="AF154" s="89"/>
+    </row>
+    <row r="155" spans="5:32">
+      <c r="V155">
+        <f t="shared" si="55"/>
+        <v>6</v>
+      </c>
+      <c r="W155" s="143"/>
+      <c r="X155" s="21"/>
+      <c r="Y155" s="21"/>
+      <c r="Z155" s="21"/>
+      <c r="AA155" s="21"/>
+      <c r="AB155" s="147">
+        <v>5</v>
+      </c>
+      <c r="AC155" s="21"/>
+      <c r="AD155" s="21"/>
+      <c r="AE155" s="21"/>
+      <c r="AF155" s="89"/>
+    </row>
+    <row r="156" spans="5:32">
+      <c r="V156">
+        <f t="shared" si="55"/>
+        <v>7</v>
+      </c>
+      <c r="W156" s="143"/>
+      <c r="X156" s="21"/>
+      <c r="Y156" s="21"/>
+      <c r="Z156" s="21"/>
+      <c r="AA156" s="21"/>
+      <c r="AB156" s="147">
+        <v>4</v>
+      </c>
+      <c r="AC156" s="21"/>
+      <c r="AD156" s="21"/>
+      <c r="AE156" s="21"/>
+      <c r="AF156" s="89"/>
+    </row>
+    <row r="157" spans="5:32">
+      <c r="V157">
+        <f t="shared" si="55"/>
+        <v>8</v>
+      </c>
+      <c r="W157" s="143"/>
+      <c r="X157" s="21"/>
+      <c r="Y157" s="21"/>
+      <c r="Z157" s="37">
+        <v>1</v>
+      </c>
+      <c r="AA157" s="147">
+        <v>2</v>
+      </c>
+      <c r="AB157" s="147">
+        <v>3</v>
+      </c>
+      <c r="AC157" s="21"/>
+      <c r="AD157" s="21"/>
+      <c r="AE157" s="21"/>
+      <c r="AF157" s="89"/>
+    </row>
+    <row r="158" spans="5:32">
+      <c r="V158">
+        <f t="shared" si="55"/>
+        <v>9</v>
+      </c>
+      <c r="W158" s="144"/>
+      <c r="X158" s="183" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y158" s="2"/>
+      <c r="Z158" s="2"/>
+      <c r="AA158" s="2"/>
+      <c r="AB158" s="2"/>
+      <c r="AC158" s="2"/>
+      <c r="AD158" s="2"/>
+      <c r="AE158" s="2"/>
+      <c r="AF158" s="113"/>
+    </row>
+    <row r="160" spans="5:32">
+      <c r="V160" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="162" spans="20:38">
+      <c r="W162" s="2">
+        <v>0</v>
+      </c>
+      <c r="X162" s="2">
+        <f t="shared" ref="X162" si="56">W162+1</f>
+        <v>1</v>
+      </c>
+      <c r="Y162" s="2">
+        <f t="shared" ref="Y162" si="57">X162+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z162" s="2">
+        <f t="shared" ref="Z162" si="58">Y162+1</f>
+        <v>3</v>
+      </c>
+      <c r="AA162" s="2">
+        <f t="shared" ref="AA162" si="59">Z162+1</f>
+        <v>4</v>
+      </c>
+      <c r="AB162" s="2">
+        <f t="shared" ref="AB162" si="60">AA162+1</f>
+        <v>5</v>
+      </c>
+      <c r="AC162" s="2">
+        <f t="shared" ref="AC162" si="61">AB162+1</f>
+        <v>6</v>
+      </c>
+      <c r="AD162" s="2">
+        <f t="shared" ref="AD162" si="62">AC162+1</f>
+        <v>7</v>
+      </c>
+      <c r="AE162" s="2">
+        <f t="shared" ref="AE162" si="63">AD162+1</f>
+        <v>8</v>
+      </c>
+      <c r="AF162" s="2">
+        <f t="shared" ref="AF162" si="64">AE162+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="20:38">
+      <c r="V163">
+        <v>0</v>
+      </c>
+      <c r="W163" s="196"/>
+      <c r="X163" s="192"/>
+      <c r="Y163" s="192"/>
+      <c r="Z163" s="192"/>
+      <c r="AA163" s="192"/>
+      <c r="AB163" s="192"/>
+      <c r="AC163" s="192"/>
+      <c r="AD163" s="192"/>
+      <c r="AE163" s="192"/>
+      <c r="AF163" s="194"/>
+    </row>
+    <row r="164" spans="20:38">
+      <c r="T164" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V164">
+        <f t="shared" ref="V164:V172" si="65">V163+1</f>
+        <v>1</v>
+      </c>
+      <c r="W164" s="197"/>
+      <c r="X164" s="193"/>
+      <c r="Y164" s="193"/>
+      <c r="Z164" s="193"/>
+      <c r="AA164" s="193"/>
+      <c r="AB164" s="193"/>
+      <c r="AC164" s="193"/>
+      <c r="AD164" s="193"/>
+      <c r="AE164" s="193"/>
+      <c r="AF164" s="195"/>
+    </row>
+    <row r="165" spans="20:38">
+      <c r="T165" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V165">
+        <f t="shared" si="65"/>
+        <v>2</v>
+      </c>
+      <c r="W165" s="197"/>
+      <c r="X165" s="193"/>
+      <c r="Y165" s="193"/>
+      <c r="Z165" s="193"/>
+      <c r="AA165" s="193"/>
+      <c r="AB165" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC165" s="21"/>
+      <c r="AD165" s="21"/>
+      <c r="AE165" s="21"/>
+      <c r="AF165" s="89"/>
+    </row>
+    <row r="166" spans="20:38" ht="15" thickBot="1">
+      <c r="T166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V166">
+        <f t="shared" si="65"/>
+        <v>3</v>
+      </c>
+      <c r="W166" s="197"/>
+      <c r="X166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y166" s="74"/>
+      <c r="Z166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE166" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF166" s="141" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ166" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="167" spans="20:38">
+      <c r="T167" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V167">
+        <f t="shared" si="65"/>
+        <v>4</v>
+      </c>
+      <c r="W167" s="197"/>
+      <c r="X167" s="17"/>
+      <c r="Y167" s="187"/>
+      <c r="Z167" s="188"/>
+      <c r="AA167" s="188"/>
+      <c r="AB167" s="188"/>
+      <c r="AC167" s="188"/>
+      <c r="AD167" s="188"/>
+      <c r="AE167" s="188"/>
+      <c r="AF167" s="189"/>
+      <c r="AJ167" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="168" spans="20:38">
+      <c r="T168" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V168">
+        <f t="shared" si="65"/>
+        <v>5</v>
+      </c>
+      <c r="W168" s="197"/>
+      <c r="X168" s="17"/>
+      <c r="Y168" s="20"/>
+      <c r="Z168" s="21"/>
+      <c r="AA168" s="21"/>
+      <c r="AB168" s="21"/>
+      <c r="AC168" s="21"/>
+      <c r="AD168" s="21"/>
+      <c r="AE168" s="21"/>
+      <c r="AF168" s="190"/>
+      <c r="AK168" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="169" spans="20:38">
+      <c r="T169" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V169">
+        <f t="shared" si="65"/>
+        <v>6</v>
+      </c>
+      <c r="W169" s="197"/>
+      <c r="X169" s="17"/>
+      <c r="Y169" s="20"/>
+      <c r="Z169" s="21"/>
+      <c r="AA169" s="21"/>
+      <c r="AB169" s="21"/>
+      <c r="AC169" s="21"/>
+      <c r="AD169" s="21"/>
+      <c r="AE169" s="21"/>
+      <c r="AF169" s="190"/>
+    </row>
+    <row r="170" spans="20:38">
+      <c r="T170" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V170">
+        <f t="shared" si="65"/>
+        <v>7</v>
+      </c>
+      <c r="W170" s="197"/>
+      <c r="X170" s="17"/>
+      <c r="Y170" s="20"/>
+      <c r="Z170" s="21"/>
+      <c r="AA170" s="21"/>
+      <c r="AB170" s="21"/>
+      <c r="AC170" s="21"/>
+      <c r="AD170" s="21"/>
+      <c r="AE170" s="21"/>
+      <c r="AF170" s="190"/>
+    </row>
+    <row r="171" spans="20:38" ht="15" thickBot="1">
+      <c r="T171" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V171">
+        <f t="shared" si="65"/>
+        <v>8</v>
+      </c>
+      <c r="W171" s="197"/>
+      <c r="X171" s="17"/>
+      <c r="Y171" s="22"/>
+      <c r="Z171" s="23"/>
+      <c r="AA171" s="23"/>
+      <c r="AB171" s="23"/>
+      <c r="AC171" s="23"/>
+      <c r="AD171" s="23"/>
+      <c r="AE171" s="23"/>
+      <c r="AF171" s="191"/>
+      <c r="AL171" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="172" spans="20:38">
+      <c r="V172">
+        <f t="shared" si="65"/>
+        <v>9</v>
+      </c>
+      <c r="W172" s="198"/>
+      <c r="X172" s="199"/>
+      <c r="Y172" s="199"/>
+      <c r="Z172" s="199"/>
+      <c r="AA172" s="199"/>
+      <c r="AB172" s="199"/>
+      <c r="AC172" s="199"/>
+      <c r="AD172" s="199"/>
+      <c r="AE172" s="199"/>
+      <c r="AF172" s="183" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL172" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="174" spans="20:38">
+      <c r="W174" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="175" spans="20:38">
+      <c r="W175" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="176" spans="20:38">
+      <c r="W176" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="178" spans="20:50" ht="15" thickBot="1">
+      <c r="W178" s="2">
+        <v>0</v>
+      </c>
+      <c r="X178" s="2">
+        <f t="shared" ref="X178" si="66">W178+1</f>
+        <v>1</v>
+      </c>
+      <c r="Y178" s="2">
+        <f t="shared" ref="Y178" si="67">X178+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z178" s="2">
+        <f t="shared" ref="Z178" si="68">Y178+1</f>
+        <v>3</v>
+      </c>
+      <c r="AA178" s="2">
+        <f t="shared" ref="AA178" si="69">Z178+1</f>
+        <v>4</v>
+      </c>
+      <c r="AB178" s="2">
+        <f t="shared" ref="AB178" si="70">AA178+1</f>
+        <v>5</v>
+      </c>
+      <c r="AC178" s="2">
+        <f t="shared" ref="AC178" si="71">AB178+1</f>
+        <v>6</v>
+      </c>
+      <c r="AD178" s="2">
+        <f t="shared" ref="AD178" si="72">AC178+1</f>
+        <v>7</v>
+      </c>
+      <c r="AE178" s="2">
+        <f t="shared" ref="AE178" si="73">AD178+1</f>
+        <v>8</v>
+      </c>
+      <c r="AF178" s="2">
+        <f t="shared" ref="AF178" si="74">AE178+1</f>
+        <v>9</v>
+      </c>
+      <c r="AL178" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM178" s="21">
+        <f t="shared" ref="AM178" si="75">AL178+1</f>
+        <v>1</v>
+      </c>
+      <c r="AN178" s="21">
+        <f t="shared" ref="AN178" si="76">AM178+1</f>
+        <v>2</v>
+      </c>
+      <c r="AO178" s="21">
+        <f t="shared" ref="AO178" si="77">AN178+1</f>
+        <v>3</v>
+      </c>
+      <c r="AP178" s="21">
+        <f t="shared" ref="AP178" si="78">AO178+1</f>
+        <v>4</v>
+      </c>
+      <c r="AQ178" s="21">
+        <f t="shared" ref="AQ178" si="79">AP178+1</f>
+        <v>5</v>
+      </c>
+      <c r="AR178" s="21">
+        <f t="shared" ref="AR178" si="80">AQ178+1</f>
+        <v>6</v>
+      </c>
+      <c r="AS178" s="21">
+        <f t="shared" ref="AS178" si="81">AR178+1</f>
+        <v>7</v>
+      </c>
+      <c r="AT178" s="21">
+        <f t="shared" ref="AT178" si="82">AS178+1</f>
+        <v>8</v>
+      </c>
+      <c r="AU178" s="21">
+        <f t="shared" ref="AU178" si="83">AT178+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="20:50">
+      <c r="V179">
+        <v>0</v>
+      </c>
+      <c r="W179" s="196"/>
+      <c r="X179" s="192"/>
+      <c r="Y179" s="192"/>
+      <c r="Z179" s="192"/>
+      <c r="AA179" s="192"/>
+      <c r="AB179" s="192"/>
+      <c r="AC179" s="192"/>
+      <c r="AD179" s="192"/>
+      <c r="AE179" s="192"/>
+      <c r="AF179" s="194"/>
+      <c r="AK179">
+        <v>0</v>
+      </c>
+      <c r="AL179" s="200"/>
+      <c r="AM179" s="121"/>
+      <c r="AN179" s="122"/>
+      <c r="AO179" s="122"/>
+      <c r="AP179" s="122"/>
+      <c r="AQ179" s="122"/>
+      <c r="AR179" s="122"/>
+      <c r="AS179" s="122"/>
+      <c r="AT179" s="122"/>
+      <c r="AU179" s="13"/>
+    </row>
+    <row r="180" spans="20:50">
+      <c r="T180" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V180">
+        <f t="shared" ref="V180:V188" si="84">V179+1</f>
+        <v>1</v>
+      </c>
+      <c r="W180" s="197"/>
+      <c r="X180" s="193"/>
+      <c r="Y180" s="193"/>
+      <c r="Z180" s="193"/>
+      <c r="AA180" s="193"/>
+      <c r="AB180" s="193"/>
+      <c r="AC180" s="193"/>
+      <c r="AD180" s="193"/>
+      <c r="AE180" s="193"/>
+      <c r="AF180" s="195"/>
+      <c r="AK180">
+        <f t="shared" ref="AK180:AK188" si="85">AK179+1</f>
+        <v>1</v>
+      </c>
+      <c r="AL180" s="81"/>
+      <c r="AM180" s="20"/>
+      <c r="AN180" s="21"/>
+      <c r="AO180" s="21"/>
+      <c r="AP180" s="21"/>
+      <c r="AQ180" s="21"/>
+      <c r="AR180" s="21"/>
+      <c r="AS180" s="21"/>
+      <c r="AT180" s="21"/>
+      <c r="AU180" s="17"/>
+      <c r="AX180" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="20:50" ht="15" thickBot="1">
+      <c r="T181" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V181">
+        <f t="shared" si="84"/>
+        <v>2</v>
+      </c>
+      <c r="W181" s="197"/>
+      <c r="X181" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y181" s="74"/>
+      <c r="Z181" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA181" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB181" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC181" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD181" s="140" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE181" s="21"/>
+      <c r="AF181" s="89"/>
+      <c r="AK181">
+        <f t="shared" si="85"/>
+        <v>2</v>
+      </c>
+      <c r="AL181" s="81"/>
+      <c r="AM181" s="20"/>
+      <c r="AN181" s="21"/>
+      <c r="AO181" s="21"/>
+      <c r="AP181" s="21"/>
+      <c r="AQ181" s="21"/>
+      <c r="AR181" s="21"/>
+      <c r="AS181" s="21"/>
+      <c r="AT181" s="21"/>
+      <c r="AU181" s="17"/>
+      <c r="AX181" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="20:50">
+      <c r="T182" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V182">
+        <f t="shared" si="84"/>
+        <v>3</v>
+      </c>
+      <c r="W182" s="197"/>
+      <c r="X182" s="17"/>
+      <c r="Y182" s="187"/>
+      <c r="Z182" s="188"/>
+      <c r="AA182" s="188"/>
+      <c r="AB182" s="188"/>
+      <c r="AC182" s="188"/>
+      <c r="AD182" s="188"/>
+      <c r="AE182" s="188"/>
+      <c r="AF182" s="189"/>
+      <c r="AK182">
+        <f t="shared" si="85"/>
+        <v>3</v>
+      </c>
+      <c r="AL182" s="81"/>
+      <c r="AM182" s="20"/>
+      <c r="AN182" s="21"/>
+      <c r="AO182" s="21"/>
+      <c r="AP182" s="21"/>
+      <c r="AQ182" s="21"/>
+      <c r="AR182" s="21"/>
+      <c r="AS182" s="21"/>
+      <c r="AT182" s="21"/>
+      <c r="AU182" s="17"/>
+      <c r="AX182" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="20:50">
+      <c r="T183" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V183">
+        <f t="shared" si="84"/>
+        <v>4</v>
+      </c>
+      <c r="W183" s="197"/>
+      <c r="X183" s="17"/>
+      <c r="AF183" s="190"/>
+      <c r="AK183">
+        <f t="shared" si="85"/>
+        <v>4</v>
+      </c>
+      <c r="AL183" s="81"/>
+      <c r="AM183" s="20"/>
+      <c r="AN183" s="21"/>
+      <c r="AO183" s="21"/>
+      <c r="AP183" s="21"/>
+      <c r="AQ183" s="21"/>
+      <c r="AR183" s="21"/>
+      <c r="AS183" s="21"/>
+      <c r="AT183" s="21"/>
+      <c r="AU183" s="17"/>
+    </row>
+    <row r="184" spans="20:50">
+      <c r="T184" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V184">
+        <f t="shared" si="84"/>
+        <v>5</v>
+      </c>
+      <c r="W184" s="197"/>
+      <c r="X184" s="17"/>
+      <c r="Y184" s="20"/>
+      <c r="Z184" s="21"/>
+      <c r="AA184" s="21"/>
+      <c r="AB184" s="21"/>
+      <c r="AC184" s="21"/>
+      <c r="AD184" s="21"/>
+      <c r="AE184" s="21"/>
+      <c r="AF184" s="190"/>
+      <c r="AK184">
+        <f t="shared" si="85"/>
+        <v>5</v>
+      </c>
+      <c r="AL184" s="81"/>
+      <c r="AM184" s="20"/>
+      <c r="AN184" s="21"/>
+      <c r="AO184" s="21"/>
+      <c r="AP184" s="21"/>
+      <c r="AQ184" s="21"/>
+      <c r="AR184" s="21"/>
+      <c r="AS184" s="21"/>
+      <c r="AT184" s="21"/>
+      <c r="AU184" s="17"/>
+    </row>
+    <row r="185" spans="20:50">
+      <c r="T185" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V185">
+        <f t="shared" si="84"/>
+        <v>6</v>
+      </c>
+      <c r="W185" s="197"/>
+      <c r="X185" s="17"/>
+      <c r="Y185" s="20"/>
+      <c r="Z185" s="21"/>
+      <c r="AA185" s="21"/>
+      <c r="AB185" s="21"/>
+      <c r="AC185" s="21"/>
+      <c r="AD185" s="21"/>
+      <c r="AE185" s="21"/>
+      <c r="AF185" s="190"/>
+      <c r="AK185">
+        <f t="shared" si="85"/>
+        <v>6</v>
+      </c>
+      <c r="AL185" s="81"/>
+      <c r="AM185" s="20"/>
+      <c r="AN185" s="21"/>
+      <c r="AO185" s="21"/>
+      <c r="AP185" s="21"/>
+      <c r="AQ185" s="21"/>
+      <c r="AR185" s="21"/>
+      <c r="AS185" s="21"/>
+      <c r="AT185" s="21"/>
+      <c r="AU185" s="17"/>
+    </row>
+    <row r="186" spans="20:50">
+      <c r="T186" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V186">
+        <f t="shared" si="84"/>
+        <v>7</v>
+      </c>
+      <c r="W186" s="197"/>
+      <c r="X186" s="17"/>
+      <c r="Y186" s="20"/>
+      <c r="Z186" s="21"/>
+      <c r="AA186" s="21"/>
+      <c r="AB186" s="21"/>
+      <c r="AC186" s="21"/>
+      <c r="AD186" s="21"/>
+      <c r="AE186" s="21"/>
+      <c r="AF186" s="190"/>
+      <c r="AK186">
+        <f t="shared" si="85"/>
+        <v>7</v>
+      </c>
+      <c r="AL186" s="81"/>
+      <c r="AM186" s="20"/>
+      <c r="AN186" s="21"/>
+      <c r="AO186" s="21"/>
+      <c r="AP186" s="21"/>
+      <c r="AQ186" s="21"/>
+      <c r="AR186" s="21"/>
+      <c r="AS186" s="21"/>
+      <c r="AT186" s="21"/>
+      <c r="AU186" s="17"/>
+    </row>
+    <row r="187" spans="20:50" ht="15" thickBot="1">
+      <c r="T187" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V187">
+        <f t="shared" si="84"/>
+        <v>8</v>
+      </c>
+      <c r="W187" s="197"/>
+      <c r="X187" s="17"/>
+      <c r="Y187" s="22"/>
+      <c r="Z187" s="23"/>
+      <c r="AA187" s="23"/>
+      <c r="AB187" s="23"/>
+      <c r="AC187" s="23"/>
+      <c r="AD187" s="23"/>
+      <c r="AE187" s="23"/>
+      <c r="AF187" s="191"/>
+      <c r="AK187">
+        <f t="shared" si="85"/>
+        <v>8</v>
+      </c>
+      <c r="AL187" s="81"/>
+      <c r="AM187" s="20"/>
+      <c r="AN187" s="21"/>
+      <c r="AO187" s="21"/>
+      <c r="AP187" s="21"/>
+      <c r="AQ187" s="21"/>
+      <c r="AR187" s="21"/>
+      <c r="AS187" s="21"/>
+      <c r="AT187" s="21"/>
+      <c r="AU187" s="17"/>
+    </row>
+    <row r="188" spans="20:50" ht="15" thickBot="1">
+      <c r="V188">
+        <f t="shared" si="84"/>
+        <v>9</v>
+      </c>
+      <c r="W188" s="198"/>
+      <c r="X188" s="199"/>
+      <c r="Y188" s="199"/>
+      <c r="Z188" s="199"/>
+      <c r="AA188" s="199"/>
+      <c r="AB188" s="199"/>
+      <c r="AC188" s="199"/>
+      <c r="AD188" s="199"/>
+      <c r="AE188" s="199"/>
+      <c r="AF188" s="183" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK188">
+        <f t="shared" si="85"/>
+        <v>9</v>
+      </c>
+      <c r="AL188" s="112"/>
+      <c r="AM188" s="22"/>
+      <c r="AN188" s="23"/>
+      <c r="AO188" s="23"/>
+      <c r="AP188" s="23"/>
+      <c r="AQ188" s="23"/>
+      <c r="AR188" s="23"/>
+      <c r="AS188" s="23"/>
+      <c r="AT188" s="23"/>
+      <c r="AU188" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working solution (Hamiltonia Cycle and short cuts) for cases 1 and 3. Case 2  follows.
</commit_message>
<xml_diff>
--- a/Snake/Documents/Helper.xlsx
+++ b/Snake/Documents/Helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Visual Studio Projects\Visual Studio 2019\Projetcs\Snake\Snake\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A02DE4-1B3C-4059-9051-AE26EF79C8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F614F2-0AB0-41D8-B86D-09C2F6101166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{43A73AA5-ABFD-421F-BFC1-09D3FBCE3DF0}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3685" uniqueCount="183">
   <si>
     <t>Hoehe</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>appl im fett umrahmten bereich ist.</t>
+  </si>
+  <si>
+    <t>PointSequence[n] = Point [x, y];</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1596,6 +1602,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -10265,10 +10272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C7CDE-FA09-4542-9DD9-60A1EEECAB2D}">
-  <dimension ref="A2:AX188"/>
+  <dimension ref="A2:AX201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="AN174" sqref="AN174"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="AM196" sqref="AM196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -15362,7 +15369,7 @@
       <c r="F144" s="138"/>
       <c r="L144" s="89"/>
     </row>
-    <row r="145" spans="5:32" ht="15" thickBot="1">
+    <row r="145" spans="5:42" ht="15" thickBot="1">
       <c r="E145">
         <f t="shared" si="45"/>
         <v>2</v>
@@ -15390,7 +15397,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="146" spans="5:32">
+    <row r="146" spans="5:42">
       <c r="E146">
         <f t="shared" si="45"/>
         <v>3</v>
@@ -15415,7 +15422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" spans="5:32">
+    <row r="147" spans="5:42">
       <c r="E147">
         <f t="shared" si="45"/>
         <v>4</v>
@@ -15428,7 +15435,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="148" spans="5:32">
+    <row r="148" spans="5:42">
       <c r="E148">
         <f t="shared" si="45"/>
         <v>5</v>
@@ -15492,7 +15499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="5:32">
+    <row r="149" spans="5:42">
       <c r="E149">
         <f t="shared" si="45"/>
         <v>6</v>
@@ -15528,7 +15535,7 @@
       <c r="AE149" s="145"/>
       <c r="AF149" s="146"/>
     </row>
-    <row r="150" spans="5:32">
+    <row r="150" spans="5:42">
       <c r="E150" t="s">
         <v>80</v>
       </c>
@@ -15549,7 +15556,7 @@
       <c r="AE150" s="147"/>
       <c r="AF150" s="148"/>
     </row>
-    <row r="151" spans="5:32">
+    <row r="151" spans="5:42">
       <c r="V151">
         <f t="shared" si="55"/>
         <v>2</v>
@@ -15566,8 +15573,11 @@
       <c r="AD151" s="21"/>
       <c r="AE151" s="21"/>
       <c r="AF151" s="89"/>
-    </row>
-    <row r="152" spans="5:32">
+      <c r="AJ151" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="152" spans="5:42">
       <c r="V152">
         <f t="shared" si="55"/>
         <v>3</v>
@@ -15584,8 +15594,17 @@
       <c r="AD152" s="21"/>
       <c r="AE152" s="21"/>
       <c r="AF152" s="89"/>
-    </row>
-    <row r="153" spans="5:32">
+      <c r="AJ152" t="s">
+        <v>182</v>
+      </c>
+      <c r="AN152" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP152" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="153" spans="5:42">
       <c r="V153">
         <f t="shared" si="55"/>
         <v>4</v>
@@ -15602,8 +15621,17 @@
       <c r="AD153" s="21"/>
       <c r="AE153" s="21"/>
       <c r="AF153" s="89"/>
-    </row>
-    <row r="154" spans="5:32">
+      <c r="AJ153">
+        <v>0</v>
+      </c>
+      <c r="AN153">
+        <v>0</v>
+      </c>
+      <c r="AP153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="5:42">
       <c r="V154">
         <f t="shared" si="55"/>
         <v>5</v>
@@ -15620,8 +15648,17 @@
       <c r="AD154" s="21"/>
       <c r="AE154" s="21"/>
       <c r="AF154" s="89"/>
-    </row>
-    <row r="155" spans="5:32">
+      <c r="AJ154">
+        <v>1</v>
+      </c>
+      <c r="AN154">
+        <v>0</v>
+      </c>
+      <c r="AP154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="5:42">
       <c r="V155">
         <f t="shared" si="55"/>
         <v>6</v>
@@ -15638,8 +15675,17 @@
       <c r="AD155" s="21"/>
       <c r="AE155" s="21"/>
       <c r="AF155" s="89"/>
-    </row>
-    <row r="156" spans="5:32">
+      <c r="AJ155">
+        <v>2</v>
+      </c>
+      <c r="AN155">
+        <v>0</v>
+      </c>
+      <c r="AP155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="5:42">
       <c r="V156">
         <f t="shared" si="55"/>
         <v>7</v>
@@ -15656,8 +15702,41 @@
       <c r="AD156" s="21"/>
       <c r="AE156" s="21"/>
       <c r="AF156" s="89"/>
-    </row>
-    <row r="157" spans="5:32">
+      <c r="AJ156">
+        <v>3</v>
+      </c>
+      <c r="AN156">
+        <v>0</v>
+      </c>
+      <c r="AP156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="5:42" ht="15" thickBot="1">
+      <c r="G157" s="21">
+        <v>0</v>
+      </c>
+      <c r="H157" s="21">
+        <f t="shared" ref="H157" si="56">G157+1</f>
+        <v>1</v>
+      </c>
+      <c r="I157" s="21">
+        <f t="shared" ref="I157" si="57">H157+1</f>
+        <v>2</v>
+      </c>
+      <c r="J157" s="21">
+        <f t="shared" ref="J157" si="58">I157+1</f>
+        <v>3</v>
+      </c>
+      <c r="K157" s="21">
+        <f t="shared" ref="K157" si="59">J157+1</f>
+        <v>4</v>
+      </c>
+      <c r="L157" s="21">
+        <f t="shared" ref="L157" si="60">K157+1</f>
+        <v>5</v>
+      </c>
+      <c r="M157" s="21"/>
       <c r="V157">
         <f t="shared" si="55"/>
         <v>8</v>
@@ -15678,8 +15757,38 @@
       <c r="AD157" s="21"/>
       <c r="AE157" s="21"/>
       <c r="AF157" s="89"/>
-    </row>
-    <row r="158" spans="5:32">
+      <c r="AJ157">
+        <v>4</v>
+      </c>
+      <c r="AN157">
+        <v>0</v>
+      </c>
+      <c r="AP157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="5:42">
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158" s="121">
+        <v>0</v>
+      </c>
+      <c r="H158" s="122">
+        <v>35</v>
+      </c>
+      <c r="I158" s="122">
+        <v>34</v>
+      </c>
+      <c r="J158" s="122">
+        <v>33</v>
+      </c>
+      <c r="K158" s="122">
+        <v>32</v>
+      </c>
+      <c r="L158" s="13">
+        <v>31</v>
+      </c>
       <c r="V158">
         <f t="shared" si="55"/>
         <v>9</v>
@@ -15697,53 +15806,167 @@
       <c r="AE158" s="2"/>
       <c r="AF158" s="113"/>
     </row>
-    <row r="160" spans="5:32">
+    <row r="159" spans="5:42">
+      <c r="F159">
+        <f t="shared" ref="F159:F164" si="61">F158+1</f>
+        <v>1</v>
+      </c>
+      <c r="G159" s="20">
+        <v>1</v>
+      </c>
+      <c r="H159" s="21">
+        <v>26</v>
+      </c>
+      <c r="I159" s="21">
+        <v>27</v>
+      </c>
+      <c r="J159" s="97">
+        <v>28</v>
+      </c>
+      <c r="K159" s="97">
+        <v>29</v>
+      </c>
+      <c r="L159" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="5:42">
+      <c r="F160">
+        <f t="shared" si="61"/>
+        <v>2</v>
+      </c>
+      <c r="G160" s="20">
+        <v>2</v>
+      </c>
+      <c r="H160" s="21">
+        <v>25</v>
+      </c>
+      <c r="I160" s="21">
+        <v>24</v>
+      </c>
+      <c r="J160" s="21">
+        <v>23</v>
+      </c>
+      <c r="K160" s="21">
+        <v>22</v>
+      </c>
+      <c r="L160" s="17">
+        <v>21</v>
+      </c>
       <c r="V160" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="162" spans="20:38">
+    <row r="161" spans="6:38">
+      <c r="F161">
+        <f t="shared" si="61"/>
+        <v>3</v>
+      </c>
+      <c r="G161" s="20">
+        <v>3</v>
+      </c>
+      <c r="H161" s="21">
+        <v>16</v>
+      </c>
+      <c r="I161" s="21">
+        <v>17</v>
+      </c>
+      <c r="J161" s="97">
+        <v>18</v>
+      </c>
+      <c r="K161" s="97">
+        <v>19</v>
+      </c>
+      <c r="L161" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="6:38">
+      <c r="F162">
+        <f t="shared" si="61"/>
+        <v>4</v>
+      </c>
+      <c r="G162" s="20">
+        <v>4</v>
+      </c>
+      <c r="H162" s="21">
+        <v>15</v>
+      </c>
+      <c r="I162" s="21">
+        <v>14</v>
+      </c>
+      <c r="J162" s="21">
+        <v>13</v>
+      </c>
+      <c r="K162" s="21">
+        <v>12</v>
+      </c>
+      <c r="L162" s="17">
+        <v>11</v>
+      </c>
       <c r="W162" s="2">
         <v>0</v>
       </c>
       <c r="X162" s="2">
-        <f t="shared" ref="X162" si="56">W162+1</f>
+        <f t="shared" ref="X162" si="62">W162+1</f>
         <v>1</v>
       </c>
       <c r="Y162" s="2">
-        <f t="shared" ref="Y162" si="57">X162+1</f>
+        <f t="shared" ref="Y162" si="63">X162+1</f>
         <v>2</v>
       </c>
       <c r="Z162" s="2">
-        <f t="shared" ref="Z162" si="58">Y162+1</f>
+        <f t="shared" ref="Z162" si="64">Y162+1</f>
         <v>3</v>
       </c>
       <c r="AA162" s="2">
-        <f t="shared" ref="AA162" si="59">Z162+1</f>
+        <f t="shared" ref="AA162" si="65">Z162+1</f>
         <v>4</v>
       </c>
       <c r="AB162" s="2">
-        <f t="shared" ref="AB162" si="60">AA162+1</f>
+        <f t="shared" ref="AB162" si="66">AA162+1</f>
         <v>5</v>
       </c>
       <c r="AC162" s="2">
-        <f t="shared" ref="AC162" si="61">AB162+1</f>
+        <f t="shared" ref="AC162" si="67">AB162+1</f>
         <v>6</v>
       </c>
       <c r="AD162" s="2">
-        <f t="shared" ref="AD162" si="62">AC162+1</f>
+        <f t="shared" ref="AD162" si="68">AC162+1</f>
         <v>7</v>
       </c>
       <c r="AE162" s="2">
-        <f t="shared" ref="AE162" si="63">AD162+1</f>
+        <f t="shared" ref="AE162" si="69">AD162+1</f>
         <v>8</v>
       </c>
       <c r="AF162" s="2">
-        <f t="shared" ref="AF162" si="64">AE162+1</f>
+        <f t="shared" ref="AF162" si="70">AE162+1</f>
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="20:38">
+    <row r="163" spans="6:38">
+      <c r="F163">
+        <f t="shared" si="61"/>
+        <v>5</v>
+      </c>
+      <c r="G163" s="20">
+        <v>5</v>
+      </c>
+      <c r="H163" s="21">
+        <v>6</v>
+      </c>
+      <c r="I163" s="21">
+        <v>7</v>
+      </c>
+      <c r="J163" s="21">
+        <v>8</v>
+      </c>
+      <c r="K163" s="21">
+        <v>9</v>
+      </c>
+      <c r="L163" s="17">
+        <v>10</v>
+      </c>
       <c r="V163">
         <v>0</v>
       </c>
@@ -15758,12 +15981,12 @@
       <c r="AE163" s="192"/>
       <c r="AF163" s="194"/>
     </row>
-    <row r="164" spans="20:38">
+    <row r="164" spans="6:38">
       <c r="T164" s="16" t="s">
         <v>17</v>
       </c>
       <c r="V164">
-        <f t="shared" ref="V164:V172" si="65">V163+1</f>
+        <f t="shared" ref="V164:V172" si="71">V163+1</f>
         <v>1</v>
       </c>
       <c r="W164" s="197"/>
@@ -15777,12 +16000,12 @@
       <c r="AE164" s="193"/>
       <c r="AF164" s="195"/>
     </row>
-    <row r="165" spans="20:38">
+    <row r="165" spans="6:38">
       <c r="T165" s="19" t="s">
         <v>16</v>
       </c>
       <c r="V165">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>2</v>
       </c>
       <c r="W165" s="197"/>
@@ -15798,12 +16021,12 @@
       <c r="AE165" s="21"/>
       <c r="AF165" s="89"/>
     </row>
-    <row r="166" spans="20:38" ht="15" thickBot="1">
+    <row r="166" spans="6:38" ht="15" thickBot="1">
       <c r="T166" s="16" t="s">
         <v>17</v>
       </c>
       <c r="V166">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>3</v>
       </c>
       <c r="W166" s="197"/>
@@ -15836,12 +16059,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="167" spans="20:38">
+    <row r="167" spans="6:38">
       <c r="T167" s="19" t="s">
         <v>16</v>
       </c>
       <c r="V167">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>4</v>
       </c>
       <c r="W167" s="197"/>
@@ -15858,12 +16081,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="168" spans="20:38">
+    <row r="168" spans="6:38">
       <c r="T168" s="16" t="s">
         <v>17</v>
       </c>
       <c r="V168">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>5</v>
       </c>
       <c r="W168" s="197"/>
@@ -15880,12 +16103,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="169" spans="20:38">
+    <row r="169" spans="6:38">
       <c r="T169" s="19" t="s">
         <v>16</v>
       </c>
       <c r="V169">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>6</v>
       </c>
       <c r="W169" s="197"/>
@@ -15899,12 +16122,12 @@
       <c r="AE169" s="21"/>
       <c r="AF169" s="190"/>
     </row>
-    <row r="170" spans="20:38">
+    <row r="170" spans="6:38">
       <c r="T170" s="16" t="s">
         <v>17</v>
       </c>
       <c r="V170">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>7</v>
       </c>
       <c r="W170" s="197"/>
@@ -15918,12 +16141,12 @@
       <c r="AE170" s="21"/>
       <c r="AF170" s="190"/>
     </row>
-    <row r="171" spans="20:38" ht="15" thickBot="1">
+    <row r="171" spans="6:38" ht="15" thickBot="1">
       <c r="T171" s="19" t="s">
         <v>16</v>
       </c>
       <c r="V171">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>8</v>
       </c>
       <c r="W171" s="197"/>
@@ -15940,9 +16163,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="172" spans="20:38">
+    <row r="172" spans="6:38">
       <c r="V172">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>9</v>
       </c>
       <c r="W172" s="198"/>
@@ -15961,17 +16184,17 @@
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="20:38">
+    <row r="174" spans="6:38">
       <c r="W174" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="175" spans="20:38">
+    <row r="175" spans="6:38">
       <c r="W175" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="176" spans="20:38">
+    <row r="176" spans="6:38">
       <c r="W176" t="s">
         <v>172</v>
       </c>
@@ -15981,78 +16204,78 @@
         <v>0</v>
       </c>
       <c r="X178" s="2">
-        <f t="shared" ref="X178" si="66">W178+1</f>
+        <f t="shared" ref="X178" si="72">W178+1</f>
         <v>1</v>
       </c>
       <c r="Y178" s="2">
-        <f t="shared" ref="Y178" si="67">X178+1</f>
+        <f t="shared" ref="Y178" si="73">X178+1</f>
         <v>2</v>
       </c>
       <c r="Z178" s="2">
-        <f t="shared" ref="Z178" si="68">Y178+1</f>
+        <f t="shared" ref="Z178" si="74">Y178+1</f>
         <v>3</v>
       </c>
       <c r="AA178" s="2">
-        <f t="shared" ref="AA178" si="69">Z178+1</f>
+        <f t="shared" ref="AA178" si="75">Z178+1</f>
         <v>4</v>
       </c>
       <c r="AB178" s="2">
-        <f t="shared" ref="AB178" si="70">AA178+1</f>
+        <f t="shared" ref="AB178" si="76">AA178+1</f>
         <v>5</v>
       </c>
       <c r="AC178" s="2">
-        <f t="shared" ref="AC178" si="71">AB178+1</f>
+        <f t="shared" ref="AC178" si="77">AB178+1</f>
         <v>6</v>
       </c>
       <c r="AD178" s="2">
-        <f t="shared" ref="AD178" si="72">AC178+1</f>
+        <f t="shared" ref="AD178" si="78">AC178+1</f>
         <v>7</v>
       </c>
       <c r="AE178" s="2">
-        <f t="shared" ref="AE178" si="73">AD178+1</f>
+        <f t="shared" ref="AE178" si="79">AD178+1</f>
         <v>8</v>
       </c>
       <c r="AF178" s="2">
-        <f t="shared" ref="AF178" si="74">AE178+1</f>
+        <f t="shared" ref="AF178" si="80">AE178+1</f>
         <v>9</v>
       </c>
       <c r="AL178" s="2">
         <v>0</v>
       </c>
       <c r="AM178" s="21">
-        <f t="shared" ref="AM178" si="75">AL178+1</f>
+        <f t="shared" ref="AM178" si="81">AL178+1</f>
         <v>1</v>
       </c>
       <c r="AN178" s="21">
-        <f t="shared" ref="AN178" si="76">AM178+1</f>
+        <f t="shared" ref="AN178" si="82">AM178+1</f>
         <v>2</v>
       </c>
       <c r="AO178" s="21">
-        <f t="shared" ref="AO178" si="77">AN178+1</f>
+        <f t="shared" ref="AO178" si="83">AN178+1</f>
         <v>3</v>
       </c>
       <c r="AP178" s="21">
-        <f t="shared" ref="AP178" si="78">AO178+1</f>
+        <f t="shared" ref="AP178" si="84">AO178+1</f>
         <v>4</v>
       </c>
       <c r="AQ178" s="21">
-        <f t="shared" ref="AQ178" si="79">AP178+1</f>
+        <f t="shared" ref="AQ178" si="85">AP178+1</f>
         <v>5</v>
       </c>
       <c r="AR178" s="21">
-        <f t="shared" ref="AR178" si="80">AQ178+1</f>
+        <f t="shared" ref="AR178" si="86">AQ178+1</f>
         <v>6</v>
       </c>
       <c r="AS178" s="21">
-        <f t="shared" ref="AS178" si="81">AR178+1</f>
+        <f t="shared" ref="AS178" si="87">AR178+1</f>
         <v>7</v>
       </c>
       <c r="AT178" s="21">
-        <f t="shared" ref="AT178" si="82">AS178+1</f>
+        <f t="shared" ref="AT178" si="88">AS178+1</f>
         <v>8</v>
       </c>
       <c r="AU178" s="21">
-        <f t="shared" ref="AU178" si="83">AT178+1</f>
+        <f t="shared" ref="AU178" si="89">AT178+1</f>
         <v>9</v>
       </c>
     </row>
@@ -16073,7 +16296,7 @@
       <c r="AK179">
         <v>0</v>
       </c>
-      <c r="AL179" s="200"/>
+      <c r="AL179" s="201"/>
       <c r="AM179" s="121"/>
       <c r="AN179" s="122"/>
       <c r="AO179" s="122"/>
@@ -16089,7 +16312,7 @@
         <v>17</v>
       </c>
       <c r="V180">
-        <f t="shared" ref="V180:V188" si="84">V179+1</f>
+        <f t="shared" ref="V180:V188" si="90">V179+1</f>
         <v>1</v>
       </c>
       <c r="W180" s="197"/>
@@ -16103,7 +16326,7 @@
       <c r="AE180" s="193"/>
       <c r="AF180" s="195"/>
       <c r="AK180">
-        <f t="shared" ref="AK180:AK188" si="85">AK179+1</f>
+        <f t="shared" ref="AK180:AK188" si="91">AK179+1</f>
         <v>1</v>
       </c>
       <c r="AL180" s="81"/>
@@ -16125,7 +16348,7 @@
         <v>16</v>
       </c>
       <c r="V181">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>2</v>
       </c>
       <c r="W181" s="197"/>
@@ -16151,7 +16374,7 @@
       <c r="AE181" s="21"/>
       <c r="AF181" s="89"/>
       <c r="AK181">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>2</v>
       </c>
       <c r="AL181" s="81"/>
@@ -16173,7 +16396,7 @@
         <v>17</v>
       </c>
       <c r="V182">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>3</v>
       </c>
       <c r="W182" s="197"/>
@@ -16187,7 +16410,7 @@
       <c r="AE182" s="188"/>
       <c r="AF182" s="189"/>
       <c r="AK182">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>3</v>
       </c>
       <c r="AL182" s="81"/>
@@ -16209,14 +16432,14 @@
         <v>16</v>
       </c>
       <c r="V183">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>4</v>
       </c>
       <c r="W183" s="197"/>
       <c r="X183" s="17"/>
       <c r="AF183" s="190"/>
       <c r="AK183">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>4</v>
       </c>
       <c r="AL183" s="81"/>
@@ -16235,7 +16458,7 @@
         <v>17</v>
       </c>
       <c r="V184">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>5</v>
       </c>
       <c r="W184" s="197"/>
@@ -16249,7 +16472,7 @@
       <c r="AE184" s="21"/>
       <c r="AF184" s="190"/>
       <c r="AK184">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>5</v>
       </c>
       <c r="AL184" s="81"/>
@@ -16268,7 +16491,7 @@
         <v>16</v>
       </c>
       <c r="V185">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>6</v>
       </c>
       <c r="W185" s="197"/>
@@ -16282,7 +16505,7 @@
       <c r="AE185" s="21"/>
       <c r="AF185" s="190"/>
       <c r="AK185">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>6</v>
       </c>
       <c r="AL185" s="81"/>
@@ -16301,7 +16524,7 @@
         <v>17</v>
       </c>
       <c r="V186">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>7</v>
       </c>
       <c r="W186" s="197"/>
@@ -16315,7 +16538,7 @@
       <c r="AE186" s="21"/>
       <c r="AF186" s="190"/>
       <c r="AK186">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>7</v>
       </c>
       <c r="AL186" s="81"/>
@@ -16334,7 +16557,7 @@
         <v>16</v>
       </c>
       <c r="V187">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>8</v>
       </c>
       <c r="W187" s="197"/>
@@ -16348,7 +16571,7 @@
       <c r="AE187" s="23"/>
       <c r="AF187" s="191"/>
       <c r="AK187">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>8</v>
       </c>
       <c r="AL187" s="81"/>
@@ -16364,7 +16587,7 @@
     </row>
     <row r="188" spans="20:50" ht="15" thickBot="1">
       <c r="V188">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>9</v>
       </c>
       <c r="W188" s="198"/>
@@ -16380,7 +16603,7 @@
         <v>164</v>
       </c>
       <c r="AK188">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>9</v>
       </c>
       <c r="AL188" s="112"/>
@@ -16393,6 +16616,232 @@
       <c r="AS188" s="23"/>
       <c r="AT188" s="23"/>
       <c r="AU188" s="24"/>
+    </row>
+    <row r="191" spans="20:50">
+      <c r="W191" s="21">
+        <v>0</v>
+      </c>
+      <c r="X191" s="21">
+        <f t="shared" ref="X191" si="92">W191+1</f>
+        <v>1</v>
+      </c>
+      <c r="Y191" s="21">
+        <f t="shared" ref="Y191" si="93">X191+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z191" s="21">
+        <f t="shared" ref="Z191" si="94">Y191+1</f>
+        <v>3</v>
+      </c>
+      <c r="AA191" s="21">
+        <f t="shared" ref="AA191" si="95">Z191+1</f>
+        <v>4</v>
+      </c>
+      <c r="AB191" s="21">
+        <f t="shared" ref="AB191" si="96">AA191+1</f>
+        <v>5</v>
+      </c>
+      <c r="AC191" s="21">
+        <f t="shared" ref="AC191" si="97">AB191+1</f>
+        <v>6</v>
+      </c>
+      <c r="AD191" s="21">
+        <f t="shared" ref="AD191" si="98">AC191+1</f>
+        <v>7</v>
+      </c>
+      <c r="AE191" s="21">
+        <f t="shared" ref="AE191" si="99">AD191+1</f>
+        <v>8</v>
+      </c>
+      <c r="AF191" s="21">
+        <f t="shared" ref="AF191" si="100">AE191+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="192" spans="20:50">
+      <c r="V192">
+        <v>0</v>
+      </c>
+      <c r="W192" s="137"/>
+      <c r="X192" s="109"/>
+      <c r="Y192" s="109"/>
+      <c r="Z192" s="109"/>
+      <c r="AA192" s="109"/>
+      <c r="AB192" s="109"/>
+      <c r="AC192" s="109"/>
+      <c r="AD192" s="109"/>
+      <c r="AE192" s="109"/>
+      <c r="AF192" s="110"/>
+    </row>
+    <row r="193" spans="20:32">
+      <c r="T193" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V193">
+        <f t="shared" ref="V193:V201" si="101">V192+1</f>
+        <v>1</v>
+      </c>
+      <c r="W193" s="138"/>
+      <c r="X193" s="21"/>
+      <c r="Y193" s="21"/>
+      <c r="Z193" s="21"/>
+      <c r="AA193" s="21"/>
+      <c r="AB193" s="21"/>
+      <c r="AC193" s="21"/>
+      <c r="AD193" s="21"/>
+      <c r="AE193" s="21"/>
+      <c r="AF193" s="89"/>
+    </row>
+    <row r="194" spans="20:32">
+      <c r="T194" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V194">
+        <f t="shared" si="101"/>
+        <v>2</v>
+      </c>
+      <c r="W194" s="138"/>
+      <c r="X194" s="21"/>
+      <c r="Y194" s="21"/>
+      <c r="Z194" s="21"/>
+      <c r="AA194" s="21"/>
+      <c r="AB194" s="21"/>
+      <c r="AC194" s="21"/>
+      <c r="AD194" s="21"/>
+      <c r="AE194" s="21"/>
+      <c r="AF194" s="89"/>
+    </row>
+    <row r="195" spans="20:32">
+      <c r="T195" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V195">
+        <f t="shared" si="101"/>
+        <v>3</v>
+      </c>
+      <c r="W195" s="138"/>
+      <c r="X195" s="193"/>
+      <c r="Y195" s="193"/>
+      <c r="Z195" s="193"/>
+      <c r="AA195" s="193"/>
+      <c r="AB195" s="183" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC195" s="21"/>
+      <c r="AD195" s="21"/>
+      <c r="AE195" s="21"/>
+      <c r="AF195" s="89"/>
+    </row>
+    <row r="196" spans="20:32">
+      <c r="T196" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V196">
+        <f t="shared" si="101"/>
+        <v>4</v>
+      </c>
+      <c r="W196" s="138"/>
+      <c r="X196" s="193"/>
+      <c r="Y196" s="193"/>
+      <c r="Z196" s="193"/>
+      <c r="AA196" s="193"/>
+      <c r="AB196" s="193"/>
+      <c r="AC196" s="193"/>
+      <c r="AD196" s="193"/>
+      <c r="AE196" s="193"/>
+      <c r="AF196" s="195"/>
+    </row>
+    <row r="197" spans="20:32">
+      <c r="T197" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V197">
+        <f t="shared" si="101"/>
+        <v>5</v>
+      </c>
+      <c r="W197" s="138"/>
+      <c r="X197" s="21"/>
+      <c r="Y197" s="21"/>
+      <c r="Z197" s="21"/>
+      <c r="AA197" s="21"/>
+      <c r="AB197" s="21"/>
+      <c r="AC197" s="21"/>
+      <c r="AD197" s="21"/>
+      <c r="AE197" s="21"/>
+      <c r="AF197" s="89"/>
+    </row>
+    <row r="198" spans="20:32">
+      <c r="T198" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V198">
+        <f t="shared" si="101"/>
+        <v>6</v>
+      </c>
+      <c r="W198" s="138"/>
+      <c r="X198" s="21"/>
+      <c r="Y198" s="21"/>
+      <c r="Z198" s="21"/>
+      <c r="AA198" s="21"/>
+      <c r="AB198" s="21"/>
+      <c r="AC198" s="21"/>
+      <c r="AD198" s="74"/>
+      <c r="AE198" s="21"/>
+      <c r="AF198" s="89"/>
+    </row>
+    <row r="199" spans="20:32">
+      <c r="T199" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="V199">
+        <f t="shared" si="101"/>
+        <v>7</v>
+      </c>
+      <c r="W199" s="138"/>
+      <c r="X199" s="21"/>
+      <c r="Y199" s="21"/>
+      <c r="Z199" s="21"/>
+      <c r="AA199" s="21"/>
+      <c r="AB199" s="21"/>
+      <c r="AC199" s="21"/>
+      <c r="AD199" s="21"/>
+      <c r="AE199" s="21"/>
+      <c r="AF199" s="89"/>
+    </row>
+    <row r="200" spans="20:32">
+      <c r="T200" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V200">
+        <f t="shared" si="101"/>
+        <v>8</v>
+      </c>
+      <c r="W200" s="138"/>
+      <c r="X200" s="21"/>
+      <c r="Y200" s="21"/>
+      <c r="Z200" s="21"/>
+      <c r="AA200" s="21"/>
+      <c r="AB200" s="21"/>
+      <c r="AC200" s="21"/>
+      <c r="AD200" s="21"/>
+      <c r="AE200" s="21"/>
+      <c r="AF200" s="89"/>
+    </row>
+    <row r="201" spans="20:32">
+      <c r="V201">
+        <f t="shared" si="101"/>
+        <v>9</v>
+      </c>
+      <c r="W201" s="200"/>
+      <c r="X201" s="2"/>
+      <c r="Y201" s="2"/>
+      <c r="Z201" s="2"/>
+      <c r="AA201" s="2"/>
+      <c r="AB201" s="2"/>
+      <c r="AC201" s="2"/>
+      <c r="AD201" s="2"/>
+      <c r="AE201" s="2"/>
+      <c r="AF201" s="113"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Made it much faster by using "pictureBox_Paint(...)" event. - Added UI control and code to change the "wait time" at run time.
</commit_message>
<xml_diff>
--- a/Snake/Documents/Helper.xlsx
+++ b/Snake/Documents/Helper.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Visual Studio Projects\Visual Studio 2019\Projetcs\Snake\Snake\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33B5D3-3600-4496-9411-77584CEF86D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704D00A-C190-47D9-A05E-8B2410FA6A62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{43A73AA5-ABFD-421F-BFC1-09D3FBCE3DF0}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{43A73AA5-ABFD-421F-BFC1-09D3FBCE3DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="3" r:id="rId1"/>
     <sheet name="B" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="151">
   <si>
     <t>¬</t>
   </si>
@@ -350,6 +351,192 @@
   <si>
     <t>im the correct order.</t>
   </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Tail</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>4 bevorzugt, da dies direkt in den HC übergehen würde</t>
+  </si>
+  <si>
+    <t>Apple hat position (13;8)</t>
+  </si>
+  <si>
+    <t>Snake length = 4</t>
+  </si>
+  <si>
+    <t>Diese Position und nicht die des Apfels ist also die Ziel Position!</t>
+  </si>
+  <si>
+    <t>Gibt es einen Weg zu dieser Ziel Position (14; 9)?</t>
+  </si>
+  <si>
+    <t>probiere es mit dem weg zum apfel der dich in den HC einphast.</t>
+  </si>
+  <si>
+    <t>Es scheint egal zu sein,</t>
+  </si>
+  <si>
+    <t>ob diagonal oder "rechtwinklig" gegangen wird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der werg hat stets die gleiche Schrittanzahl </t>
+  </si>
+  <si>
+    <t>Punkt in der HC Abfolge, der 4 (also = snake length) Positionen vor der Apfel-Position ist lautet: (14; 9)</t>
+  </si>
+  <si>
+    <t>Hier müßten</t>
+  </si>
+  <si>
+    <t>von Varianen!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also das sich snake-head, -tail und -body exakt in der Reihenfolge befinden, </t>
+  </si>
+  <si>
+    <t>die durch den HC vorgegeben wird?</t>
+  </si>
+  <si>
+    <t>ALLE MÖGLICHEN</t>
+  </si>
+  <si>
+    <t>Also MILLIARDEN</t>
+  </si>
+  <si>
+    <t>Wege überprüft</t>
+  </si>
+  <si>
+    <t>werden.</t>
+  </si>
+  <si>
+    <t>gibt es dann zumindest noch noch einen Weg,</t>
+  </si>
+  <si>
+    <t>der dafür sorgt, dass die snake die maximale Länge erreichen kann,</t>
+  </si>
+  <si>
+    <t>die durch die Spielfeldgröße vorgegeben ist!</t>
+  </si>
+  <si>
+    <t>ja:</t>
+  </si>
+  <si>
+    <t>nein:</t>
+  </si>
+  <si>
+    <t>Ist die snake schon vollständig im HC eingephast</t>
+  </si>
+  <si>
+    <t>und</t>
+  </si>
+  <si>
+    <t>ist der Abstand zwischen snake head und Apfel kleiner oder gleich mit der snake-Länge?</t>
+  </si>
+  <si>
+    <t>Keinen shortcut berechnen, sondern HC path folgen, da ...</t>
+  </si>
+  <si>
+    <t>Frage 1:</t>
+  </si>
+  <si>
+    <t>Frage 3:</t>
+  </si>
+  <si>
+    <t>Frage 2:</t>
+  </si>
+  <si>
+    <t>um die snake komplett in den Hamiltonian Cycle (=HC) einzuphasen,</t>
+  </si>
+  <si>
+    <t>Gehe auf dem kürzesten Weg zum Apfel und verzehre ihn ...</t>
+  </si>
+  <si>
+    <t>VERMUTE, dass dieser Zusatz</t>
+  </si>
+  <si>
+    <t>ersatzlos entfernt werden muss:</t>
+  </si>
+  <si>
+    <t>Nach dem Apfelverkehr gibt es offensichtlich keinen Weg, um die snake wieder in den HC einzuphasen,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(ALSON NICHT DEM HC path folgt! Der HC path muss also ausgeschjloeen werden!) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn die Schlange direkt zum Apfel geht, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">und den Apfel verzehrt, </t>
+  </si>
+  <si>
+    <t>dabei nicht dem Weg folgt, der durch den HC definiert ist</t>
+  </si>
+  <si>
+    <t>HC path folgen wäre keine Abkürzung daher die entsprechende Bedingung, dass der zu untersuchende Weg nicht der ist, der dem HC Weg entspricht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denn es ist sichergestellt, das nach dem Apfelverzehr, die snake in den HC gephast werden kann, </t>
+  </si>
+  <si>
+    <t>denn ansonsten wäre die Frage (1) mit nein beantwortet worden.</t>
+  </si>
+  <si>
+    <t>In der hier betrachteten Situation ist die snake aber bereits im HC eingephast.</t>
+  </si>
+  <si>
+    <t>Einen shortcut zu berechnen und zu folgen würde also bedeuten,</t>
+  </si>
+  <si>
+    <t>nach dem Apfelverzehr keine Chance mehr zu haben in den HC eingephast zu werden.</t>
+  </si>
+  <si>
+    <t>Dies ist aber wichtig, denn der HC ist die Grundlage dafür, dass die snake die maximale Länge erreichen kann,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - snake nicht eingephast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - direkt zu apfel gehen, geht nicht, da snake danach nicht eingephast werden kann</t>
+  </si>
+  <si>
+    <t>Ziel muss also sein die snake in den HC einzuphasen.</t>
+  </si>
+  <si>
+    <t>aber sie sofort einzuphasen kann bedeuten das moves gemacht werden die eingespart werden können.</t>
+  </si>
+  <si>
+    <t>die snake muss ja nur, bzw. spätestens eingephast sein, wenn sie den Apfel frisst.</t>
+  </si>
+  <si>
+    <t>Hier kommt also die Länge der snake ins Spiel.</t>
+  </si>
+  <si>
+    <t>daher:</t>
+  </si>
+  <si>
+    <t>Wenn die snake also die position vor dem apfel erreicht, die der snake länge entspricht,</t>
+  </si>
+  <si>
+    <t>wird sich die snake bei diesen "snake-länge-vielen" moves eingephast haben, wenn sie den Apfel</t>
+  </si>
+  <si>
+    <t>verzehrt hat.</t>
+  </si>
+  <si>
+    <t>Gehe auf kürzestem Weg zu dieser Position</t>
+  </si>
+  <si>
+    <t>berechne einen path, so dass die Schlange, nach Abarbeitung dieses path, komplett im HC eingephast ist.</t>
+  </si>
 </sst>
 </file>
 
@@ -408,7 +595,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +659,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1041,6 +1246,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7C1CA8-4445-4A42-837E-08649278B969}">
   <dimension ref="A1:AN61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AG30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14:W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4699,8 +4915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C7CDE-FA09-4542-9DD9-60A1EEECAB2D}">
   <dimension ref="A2:BH343"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G203" sqref="G203"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5408,18 +5624,18 @@
         <v>2</v>
       </c>
       <c r="H26" s="49"/>
-      <c r="K26" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="K26">
+        <f>K25+1</f>
+        <v>4</v>
       </c>
       <c r="L26" s="48"/>
       <c r="M26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="O26" s="49"/>
-      <c r="S26" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
+      <c r="S26">
+        <f>S25+1</f>
+        <v>4</v>
       </c>
       <c r="T26" s="48"/>
       <c r="U26" s="4" t="s">
@@ -5446,9 +5662,9 @@
       <c r="I27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K27" t="e">
+      <c r="K27">
         <f>K26+1</f>
-        <v>#REF!</v>
+        <v>5</v>
       </c>
       <c r="L27" s="48"/>
       <c r="M27" s="7" t="s">
@@ -5461,9 +5677,9 @@
       <c r="P27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="S27" t="e">
+      <c r="S27">
         <f>S26+1</f>
-        <v>#REF!</v>
+        <v>5</v>
       </c>
       <c r="T27" s="48"/>
       <c r="U27" s="7" t="s">
@@ -5479,20 +5695,6 @@
       <c r="Y27" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="3:28" x14ac:dyDescent="0.4">
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="48"/>
-      <c r="K29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L29" s="48"/>
-      <c r="S29" t="s">
-        <v>6</v>
-      </c>
-      <c r="T29" s="48"/>
     </row>
     <row r="42" spans="35:47" x14ac:dyDescent="0.4">
       <c r="AJ42" s="1">
@@ -17929,11 +18131,1225 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C072AF83-E84E-4397-AB0A-928AA0C0DC6D}">
+  <dimension ref="B2:AZ89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="P90" sqref="P90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="51" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:L2" si="0">C2+1</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R2" s="140"/>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="109"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="R3" s="141"/>
+      <c r="T3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <f t="shared" ref="B4:B12" si="1">B3+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="141"/>
+      <c r="L4" s="21"/>
+      <c r="R4" s="142"/>
+      <c r="T4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="143">
+        <v>1</v>
+      </c>
+      <c r="H5" s="143">
+        <v>2</v>
+      </c>
+      <c r="I5" s="143">
+        <v>3</v>
+      </c>
+      <c r="L5" s="21"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="F6" s="143">
+        <v>1</v>
+      </c>
+      <c r="G6" s="143">
+        <v>2</v>
+      </c>
+      <c r="I6" s="143">
+        <v>4</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="R6" s="17"/>
+      <c r="T6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="F7" s="143">
+        <v>2</v>
+      </c>
+      <c r="G7" s="143">
+        <v>3</v>
+      </c>
+      <c r="H7" s="143">
+        <v>4</v>
+      </c>
+      <c r="I7" s="143">
+        <v>5</v>
+      </c>
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="F8" s="143">
+        <v>3</v>
+      </c>
+      <c r="H8" s="143">
+        <v>5</v>
+      </c>
+      <c r="I8" s="143">
+        <v>6</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="R8" s="143"/>
+      <c r="T8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="F9" s="143">
+        <v>4</v>
+      </c>
+      <c r="I9" s="143">
+        <v>7</v>
+      </c>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="F10" s="143">
+        <v>5</v>
+      </c>
+      <c r="I10" s="143">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="F11" s="143">
+        <v>6</v>
+      </c>
+      <c r="G11" s="143">
+        <v>7</v>
+      </c>
+      <c r="H11" s="143">
+        <v>8</v>
+      </c>
+      <c r="I11" s="143">
+        <v>9</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11" s="21"/>
+      <c r="N11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="31"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="AG13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.4">
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="AL17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:R18" si="2">C18+1</f>
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="109"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="29"/>
+      <c r="T19" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA19" s="145"/>
+      <c r="AC19" s="146" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD19" s="146"/>
+      <c r="AE19" s="146"/>
+    </row>
+    <row r="20" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B20">
+        <f t="shared" ref="B20:B28" si="3">B19+1</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="141"/>
+      <c r="R20" s="21"/>
+      <c r="T20" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA20" s="145"/>
+      <c r="AC20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="143">
+        <v>1</v>
+      </c>
+      <c r="H21" s="143">
+        <v>2</v>
+      </c>
+      <c r="I21" s="143">
+        <v>3</v>
+      </c>
+      <c r="J21" s="143">
+        <v>4</v>
+      </c>
+      <c r="K21" s="143">
+        <v>5</v>
+      </c>
+      <c r="L21" s="143">
+        <v>6</v>
+      </c>
+      <c r="M21" s="143">
+        <v>7</v>
+      </c>
+      <c r="N21" s="143">
+        <v>8</v>
+      </c>
+      <c r="O21" s="143">
+        <v>9</v>
+      </c>
+      <c r="R21" s="21"/>
+      <c r="T21" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA21" s="145"/>
+      <c r="AC21" t="s">
+        <v>131</v>
+      </c>
+      <c r="AZ21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B22">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="F22" s="143">
+        <v>1</v>
+      </c>
+      <c r="G22" s="143">
+        <v>2</v>
+      </c>
+      <c r="O22" s="143">
+        <v>10</v>
+      </c>
+      <c r="R22" s="21"/>
+      <c r="T22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA22" s="145"/>
+      <c r="AC22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B23">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="G23" s="143">
+        <v>3</v>
+      </c>
+      <c r="H23" s="143">
+        <v>4</v>
+      </c>
+      <c r="O23" s="143">
+        <v>11</v>
+      </c>
+      <c r="R23" s="21"/>
+      <c r="T23" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA23" s="145"/>
+      <c r="AC23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="H24" s="143">
+        <v>5</v>
+      </c>
+      <c r="I24" s="143">
+        <v>6</v>
+      </c>
+      <c r="O24" s="143">
+        <v>12</v>
+      </c>
+      <c r="R24" s="21"/>
+      <c r="T24" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA24" s="145"/>
+      <c r="AC24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="I25" s="143">
+        <v>7</v>
+      </c>
+      <c r="J25" s="143">
+        <v>8</v>
+      </c>
+      <c r="O25" s="143">
+        <v>13</v>
+      </c>
+      <c r="R25" s="21"/>
+      <c r="AC25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B26">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="J26" s="143">
+        <v>9</v>
+      </c>
+      <c r="K26" s="143">
+        <v>10</v>
+      </c>
+      <c r="O26" s="143">
+        <v>14</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="21"/>
+      <c r="AC26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B27">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="K27" s="143">
+        <v>11</v>
+      </c>
+      <c r="L27" s="143">
+        <v>12</v>
+      </c>
+      <c r="M27" s="143">
+        <v>13</v>
+      </c>
+      <c r="N27" s="143">
+        <v>14</v>
+      </c>
+      <c r="O27" s="143">
+        <v>15</v>
+      </c>
+      <c r="P27" s="17"/>
+      <c r="Q27">
+        <v>4</v>
+      </c>
+      <c r="R27" s="21"/>
+    </row>
+    <row r="28" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="B28">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="144"/>
+      <c r="R28" s="31"/>
+      <c r="AC28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="AD29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="AE30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="AE31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="2:52" x14ac:dyDescent="0.4">
+      <c r="AE32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AC34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AD35" s="146" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE35" s="146"/>
+      <c r="AF35" s="146"/>
+    </row>
+    <row r="36" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AD36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF37" s="142" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG37" s="142"/>
+      <c r="AH37" s="142"/>
+      <c r="AI37" s="142"/>
+      <c r="AJ37" s="142"/>
+      <c r="AK37" s="142"/>
+      <c r="AL37" s="142"/>
+      <c r="AM37" s="142"/>
+      <c r="AN37" s="142"/>
+      <c r="AP37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF38" s="142" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG38" s="142"/>
+      <c r="AH38" s="142"/>
+      <c r="AI38" s="142"/>
+      <c r="AJ38" s="142"/>
+      <c r="AK38" s="142"/>
+      <c r="AL38" s="142"/>
+      <c r="AM38" s="142"/>
+      <c r="AN38" s="142"/>
+      <c r="AP38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AD40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AE41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="29:42" x14ac:dyDescent="0.4">
+      <c r="AF48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AD50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE57" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="AE60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <f t="shared" ref="F61:T61" si="4">E61+1</f>
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" s="109"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="28"/>
+      <c r="Q62" s="28"/>
+      <c r="R62" s="28"/>
+      <c r="S62" s="28"/>
+      <c r="T62" s="29"/>
+      <c r="AE62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="D63">
+        <f t="shared" ref="D63:D71" si="5">D62+1</f>
+        <v>1</v>
+      </c>
+      <c r="E63" s="20"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="9"/>
+      <c r="R63" s="9"/>
+      <c r="S63" s="9"/>
+      <c r="T63" s="21"/>
+      <c r="AE63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="4:31" x14ac:dyDescent="0.4">
+      <c r="D64">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E64" s="20"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="21"/>
+      <c r="AE64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E65" s="20"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="21"/>
+      <c r="AE65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D66">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E66" s="20"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="9"/>
+      <c r="S66" s="9"/>
+      <c r="T66" s="21"/>
+      <c r="AE66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D67">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E67" s="20"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="9"/>
+      <c r="R67" s="9"/>
+      <c r="S67" s="9"/>
+      <c r="T67" s="21"/>
+      <c r="AE67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E68" s="20"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="21"/>
+      <c r="AE68" s="146" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF68" s="146"/>
+      <c r="AG68" s="146"/>
+    </row>
+    <row r="69" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="E69" s="20"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="9"/>
+      <c r="R69" s="9"/>
+      <c r="S69" s="9"/>
+      <c r="T69" s="21"/>
+      <c r="AE69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E70" s="20"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="9"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="9"/>
+      <c r="R70" s="9"/>
+      <c r="S70" s="9"/>
+      <c r="T70" s="21"/>
+      <c r="AE70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="E71" s="30"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="31"/>
+      <c r="AF71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="AE73" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="4:33" x14ac:dyDescent="0.4">
+      <c r="AF74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <f t="shared" ref="F81:T81" si="6">E81+1</f>
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82" s="147"/>
+      <c r="F82" s="55"/>
+      <c r="G82" s="55"/>
+      <c r="H82" s="55"/>
+      <c r="I82" s="55"/>
+      <c r="J82" s="56"/>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D83">
+        <f t="shared" ref="D83:D91" si="7">D82+1</f>
+        <v>1</v>
+      </c>
+      <c r="E83" s="62"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="57"/>
+      <c r="H83" s="57"/>
+      <c r="I83" s="57"/>
+      <c r="J83" s="58"/>
+    </row>
+    <row r="84" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D84">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="E84" s="62"/>
+      <c r="F84" s="57"/>
+      <c r="G84" s="57"/>
+      <c r="H84" s="57"/>
+      <c r="I84" s="57"/>
+      <c r="J84" s="58"/>
+    </row>
+    <row r="85" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D85">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="E85" s="148"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="58"/>
+    </row>
+    <row r="86" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D86">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E86" s="20"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="58"/>
+    </row>
+    <row r="87" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D87">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E87" s="20"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="58"/>
+    </row>
+    <row r="88" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D88">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="E88" s="20"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="58"/>
+    </row>
+    <row r="89" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D89">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="E89" s="149"/>
+      <c r="F89" s="60"/>
+      <c r="G89" s="60"/>
+      <c r="H89" s="60"/>
+      <c r="I89" s="60"/>
+      <c r="J89" s="150"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED405DBE-15DD-4130-B31E-6D15D7D4142D}">
   <dimension ref="C2:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -18374,7 +19790,7 @@
     </row>
     <row r="15" spans="3:26" x14ac:dyDescent="0.4">
       <c r="C15">
-        <f t="shared" ref="C15:C20" si="5">C14+1</f>
+        <f t="shared" ref="C15:C19" si="5">C14+1</f>
         <v>1</v>
       </c>
       <c r="D15" s="26" t="s">
@@ -18426,11 +19842,11 @@
       <c r="D16" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="E16" s="124" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="3" t="s">
         <v>1</v>
       </c>
@@ -18454,7 +19870,9 @@
       <c r="D17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="7" t="s">
         <v>2</v>
@@ -18485,7 +19903,9 @@
       <c r="D18" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="7" t="s">
         <v>2</v>
@@ -18516,7 +19936,9 @@
       <c r="D19" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="7" t="s">
         <v>2</v>
@@ -18548,11 +19970,9 @@
       <c r="D20" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="124" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="125"/>
-      <c r="G20" s="125"/>
+      <c r="E20" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="H20" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>